<commit_message>
feat: add loading feature
</commit_message>
<xml_diff>
--- a/suffix_data/Suffix_D03B.xlsx
+++ b/suffix_data/Suffix_D03B.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah Alfons\Python Projects\front-ub-tmmin\ai-ub-front-p2\backend\suffix_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kuliah Alfons\Toyota\front_project\front_ub_no_ms\backend\suffix_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="81">
   <si>
     <t>AA</t>
   </si>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>PARTNAME</t>
-  </si>
-  <si>
-    <t>RED GREEN</t>
   </si>
   <si>
     <t>T4</t>
@@ -743,11 +740,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA9"/>
+  <dimension ref="A1:BA7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1075,1129 +1072,807 @@
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>56</v>
+      <c r="A3" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>75</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>75</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="O3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AD3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AE3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="AF3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AG3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AH3" s="6" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="AI3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AJ3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AK3" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="AL3" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="AM3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AN3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AO3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AP3" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="AQ3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AR3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AS3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AT3" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="AU3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AV3" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="AW3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AX3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AY3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="AZ3" s="6" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="BA3" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="AA4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="AB4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="AC4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="AD4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="AE4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="AF4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="AG4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="AH4" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="AI4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AJ4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AK4" s="6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AL4" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AM4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AN4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AO4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AP4" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AQ4" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="AR4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AS4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AT4" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AU4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AV4" s="6" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AW4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AX4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AY4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AZ4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="BA4" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="X5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="Y5" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Z5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AA5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AB5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AC5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AD5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AE5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AF5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AG5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AH5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AI5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AJ5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AK5" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AL5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AM5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AN5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AO5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AP5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AQ5" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AR5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AS5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AT5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AU5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AV5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AW5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AX5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AY5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AZ5" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="BA5" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AB6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AC6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AF6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AG6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AH6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AJ6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AK6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AL6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AM6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AN6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AO6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AP6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AQ6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AR6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AS6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AT6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AU6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AV6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AW6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AX6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AY6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="AZ6" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="BA6" s="6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="W7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Y7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AB7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AC7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AD7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AE7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AF7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AG7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AH7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AI7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AJ7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AK7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AL7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AM7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AN7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AO7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AP7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AQ7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AR7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AS7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AT7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AU7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AV7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AW7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AX7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AY7" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AZ7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="BA7" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="R8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="T8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="U8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="V8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="W8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="X8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AG8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AH8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AI8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AJ8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AK8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AL8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AM8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AN8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AP8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AR8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AS8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AT8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AU8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AV8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AX8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AY8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="AZ8" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="BA8" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="R9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="U9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="V9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="W9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="X9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AA9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AK9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AL9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AM9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AO9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AP9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AQ9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AR9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AT9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AV9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AW9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AY9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="AZ9" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="BA9" s="6" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2251,7 +1926,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>62</v>
@@ -2275,7 +1950,7 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>63</v>
@@ -2295,7 +1970,7 @@
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -2307,7 +1982,7 @@
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -2319,7 +1994,7 @@
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -2331,7 +2006,7 @@
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>

</xml_diff>